<commit_message>
modele circuit avec départ et un nom
</commit_message>
<xml_diff>
--- a/Code_jeu/maps/GenerateurMap.xlsx
+++ b/Code_jeu/maps/GenerateurMap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usherbrooke-my.sharepoint.com/personal/giff1201_usherbrooke_ca/Documents/S2/projet/Projet-S2/Code_jeu/maps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\techn\OneDrive - USherbrooke\S2\projet\Projet-S2\Code_jeu\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{0CB93EEA-7747-49AD-9BD6-4973FBF48027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1170792-ECBD-45DE-A6BE-BBC3E3C7F231}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62028F5D-3DA3-4D75-9117-829750DF8A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BA35D6A-4D2B-43E3-A660-9236F0A02439}"/>
   </bookViews>
@@ -71,7 +71,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -395,7 +405,7 @@
   <dimension ref="A1:AX50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AX50" sqref="A1:AX50"/>
+      <selection activeCell="BB29" sqref="BB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4337,7 +4347,7 @@
         <v>1</v>
       </c>
       <c r="AS26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AT26">
         <v>1</v>
@@ -8005,8 +8015,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AX50">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>0</formula>
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>